<commit_message>
conclusions of missing data and new datasets including all
</commit_message>
<xml_diff>
--- a/scripts/mssing ids.xlsx
+++ b/scripts/mssing ids.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E059E4A4-2F0A-4931-BF19-787BE47E8F48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parent" sheetId="1" r:id="rId1"/>
     <sheet name="youth" sheetId="2" r:id="rId2"/>
+    <sheet name="parent &amp; youth" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">parent!$B$1:$E$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'parent &amp; youth'!$D$1:$D$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">youth!$C$1:$C$98</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="165">
   <si>
     <t>101_1</t>
   </si>
@@ -445,9 +452,6 @@
     <t>w3 complete, no w2 data. Contact logs show no evidence of completing w2</t>
   </si>
   <si>
-    <t>youth data until q186 (R_3jebHOrmpEvVusr), paent data missing</t>
-  </si>
-  <si>
     <t>youth data complete (R_10ryStLMAuTyIpH) even though it says this row is false</t>
   </si>
   <si>
@@ -488,13 +492,43 @@
   </si>
   <si>
     <t>pa w3</t>
+  </si>
+  <si>
+    <t>yellow: 95 primary caregivers</t>
+  </si>
+  <si>
+    <t>11 caregivers lost to w2</t>
+  </si>
+  <si>
+    <t>parent primary caregiver w1</t>
+  </si>
+  <si>
+    <t>youth w1</t>
+  </si>
+  <si>
+    <t>parent primary w2</t>
+  </si>
+  <si>
+    <t>youth w2</t>
+  </si>
+  <si>
+    <t>candidate for missingnes procedure</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>youth data until q186 (R_3jebHOrmpEvVusr), paRent data missing</t>
+  </si>
+  <si>
+    <t>no w2 data. Logs indicate complete assessment at home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -515,8 +549,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,6 +576,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -548,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -556,11 +621,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -835,1173 +932,1188 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:G138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="N119" sqref="N119"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" t="s">
+      <c r="F15" s="2"/>
+      <c r="G15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>31</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>31</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>36</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>39</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B54" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B55" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B56" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2"/>
+      <c r="E59" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="4" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>64</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B67" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B68" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B69" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>70</v>
+      </c>
+      <c r="D71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
+      <c r="D72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B73" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B74" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B75" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B76" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>76</v>
+      </c>
+      <c r="D77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B78" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F78" s="2"/>
+      <c r="G78" t="s">
         <v>143</v>
       </c>
-      <c r="E60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="C61" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="4" t="s">
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B79" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B80" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+      <c r="D81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B82" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B83" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B85" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B86" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>86</v>
+      </c>
+      <c r="D87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B88" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>88</v>
+      </c>
+      <c r="D89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B90" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B91" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F91" s="2"/>
+      <c r="G91" t="s">
         <v>143</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>71</v>
-      </c>
-      <c r="C72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>73</v>
-      </c>
-      <c r="C74" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>74</v>
-      </c>
-      <c r="C75" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>76</v>
-      </c>
-      <c r="C77" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>78</v>
-      </c>
-      <c r="C79" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>79</v>
-      </c>
-      <c r="C80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>80</v>
-      </c>
-      <c r="C81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>81</v>
-      </c>
-      <c r="C82" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>82</v>
-      </c>
-      <c r="C83" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>83</v>
-      </c>
-      <c r="C84" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>84</v>
-      </c>
-      <c r="C85" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>85</v>
-      </c>
-      <c r="C86" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>86</v>
-      </c>
-      <c r="C87" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>87</v>
-      </c>
-      <c r="C88" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>88</v>
-      </c>
-      <c r="C89" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>89</v>
-      </c>
-      <c r="C90" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>90</v>
-      </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E91" s="2"/>
-      <c r="F91" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B92" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C92" s="2"/>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="2"/>
+      <c r="E92" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
         <v>92</v>
       </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="2"/>
+      <c r="E93" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B94" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B95" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B96" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
         <v>96</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B98" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B99" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B100" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B101" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B102" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B103" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>132</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>102</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E103" s="2"/>
-      <c r="F103" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="E103" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F103" s="2"/>
+      <c r="G103" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B104" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
         <v>104</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
         <v>105</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B107" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
         <v>107</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B109" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B110" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B111" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C111" s="2"/>
-      <c r="D111" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E111">
+      <c r="D111" s="2"/>
+      <c r="E111" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F111" s="10">
         <v>612</v>
       </c>
-      <c r="F111" t="s">
+      <c r="G111" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
         <v>111</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B113" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B114" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
         <v>114</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B116" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
         <v>116</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B118" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B119" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B120" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>132</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="E120" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E120">
+      <c r="F120" s="10">
         <v>619</v>
       </c>
-      <c r="F120" t="s">
+      <c r="G120" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B121" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>132</v>
       </c>
-      <c r="C121" s="2"/>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="2"/>
+      <c r="E121" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F121" s="10">
+        <v>620</v>
+      </c>
+      <c r="G121" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B122" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C122" t="s">
+        <v>132</v>
+      </c>
+      <c r="D122" t="s">
+        <v>121</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B123" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D123" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B124" s="2"/>
+      <c r="C124" t="s">
+        <v>152</v>
+      </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B125" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D125" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B127" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E127" s="6"/>
+      <c r="F127" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E121">
-        <v>620</v>
-      </c>
-      <c r="F121" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>121</v>
-      </c>
-      <c r="B122" t="s">
-        <v>132</v>
-      </c>
-      <c r="C122" t="s">
-        <v>121</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>122</v>
-      </c>
-      <c r="C123" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="2"/>
-      <c r="B124" t="s">
-        <v>153</v>
-      </c>
-      <c r="C124" s="2"/>
-      <c r="D124" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>123</v>
-      </c>
-      <c r="C125" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B127" s="5"/>
-      <c r="C127" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D127" s="6"/>
-      <c r="E127" s="5" t="s">
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
         <v>155</v>
       </c>
     </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="B1:E137" xr:uid="{3C1546A2-BF81-4539-8024-42C8CDD12298}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>101</v>
       </c>
@@ -2009,7 +2121,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>102</v>
       </c>
@@ -2017,7 +2129,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>103</v>
       </c>
@@ -2025,7 +2137,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>104</v>
       </c>
@@ -2033,7 +2145,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>105</v>
       </c>
@@ -2041,7 +2153,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>106</v>
       </c>
@@ -2049,7 +2161,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>107</v>
       </c>
@@ -2057,7 +2169,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>108</v>
       </c>
@@ -2065,7 +2177,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>109</v>
       </c>
@@ -2073,20 +2185,25 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>110</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="E10" s="1">
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="3">
         <v>110</v>
       </c>
       <c r="F10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>111</v>
       </c>
@@ -2094,7 +2211,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>112</v>
       </c>
@@ -2109,7 +2226,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>113</v>
       </c>
@@ -2124,7 +2241,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>114</v>
       </c>
@@ -2132,7 +2249,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>201</v>
       </c>
@@ -2140,7 +2257,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>202</v>
       </c>
@@ -2148,7 +2265,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>203</v>
       </c>
@@ -2156,7 +2273,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>204</v>
       </c>
@@ -2164,7 +2281,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>205</v>
       </c>
@@ -2172,7 +2289,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>206</v>
       </c>
@@ -2180,7 +2297,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>207</v>
       </c>
@@ -2188,7 +2305,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>208</v>
       </c>
@@ -2196,7 +2313,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>209</v>
       </c>
@@ -2205,7 +2322,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>210</v>
       </c>
@@ -2220,7 +2337,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>211</v>
       </c>
@@ -2228,7 +2345,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>212</v>
       </c>
@@ -2236,7 +2353,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>214</v>
       </c>
@@ -2244,7 +2361,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>215</v>
       </c>
@@ -2252,7 +2369,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>216</v>
       </c>
@@ -2260,7 +2377,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>302</v>
       </c>
@@ -2268,7 +2385,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>304</v>
       </c>
@@ -2276,7 +2393,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>305</v>
       </c>
@@ -2284,7 +2401,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>306</v>
       </c>
@@ -2292,7 +2409,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>307</v>
       </c>
@@ -2300,7 +2417,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>308</v>
       </c>
@@ -2308,7 +2425,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>309</v>
       </c>
@@ -2316,7 +2433,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>310</v>
       </c>
@@ -2324,7 +2441,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>311</v>
       </c>
@@ -2332,7 +2449,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>312</v>
       </c>
@@ -2340,7 +2457,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>313</v>
       </c>
@@ -2348,7 +2465,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>314</v>
       </c>
@@ -2356,7 +2473,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>315</v>
       </c>
@@ -2364,7 +2481,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>317</v>
       </c>
@@ -2372,7 +2489,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>318</v>
       </c>
@@ -2380,7 +2497,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>401</v>
       </c>
@@ -2388,7 +2505,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>403</v>
       </c>
@@ -2396,7 +2513,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>404</v>
       </c>
@@ -2404,7 +2521,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>405</v>
       </c>
@@ -2412,16 +2529,16 @@
         <v>405</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="E48">
         <v>405</v>
       </c>
       <c r="F48" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>406</v>
       </c>
@@ -2429,20 +2546,20 @@
         <v>406</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>407</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>408</v>
       </c>
@@ -2450,16 +2567,16 @@
         <v>408</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>410</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>411</v>
       </c>
@@ -2467,7 +2584,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>412</v>
       </c>
@@ -2475,7 +2592,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>413</v>
       </c>
@@ -2483,7 +2600,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>414</v>
       </c>
@@ -2491,7 +2608,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>415</v>
       </c>
@@ -2499,7 +2616,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>416</v>
       </c>
@@ -2507,7 +2624,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>417</v>
       </c>
@@ -2515,7 +2632,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>418</v>
       </c>
@@ -2523,20 +2640,20 @@
         <v>418</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>419</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>420</v>
       </c>
@@ -2544,7 +2661,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>501</v>
       </c>
@@ -2552,7 +2669,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>502</v>
       </c>
@@ -2560,7 +2677,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>503</v>
       </c>
@@ -2568,10 +2685,10 @@
         <v>503</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C66">
         <v>504</v>
@@ -2586,7 +2703,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>505</v>
       </c>
@@ -2594,7 +2711,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>506</v>
       </c>
@@ -2602,7 +2719,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>507</v>
       </c>
@@ -2610,20 +2727,20 @@
         <v>507</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>508</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>509</v>
       </c>
@@ -2632,7 +2749,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>510</v>
       </c>
@@ -2640,7 +2757,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>511</v>
       </c>
@@ -2648,7 +2765,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>513</v>
       </c>
@@ -2656,7 +2773,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>601</v>
       </c>
@@ -2664,7 +2781,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>602</v>
       </c>
@@ -2672,7 +2789,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>603</v>
       </c>
@@ -2680,7 +2797,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>604</v>
       </c>
@@ -2688,7 +2805,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>605</v>
       </c>
@@ -2696,7 +2813,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>606</v>
       </c>
@@ -2705,11 +2822,11 @@
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>607</v>
       </c>
@@ -2717,7 +2834,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>608</v>
       </c>
@@ -2725,7 +2842,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>610</v>
       </c>
@@ -2733,7 +2850,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>611</v>
       </c>
@@ -2741,13 +2858,13 @@
         <v>611</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>612</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E85">
         <v>612</v>
@@ -2756,7 +2873,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>613</v>
       </c>
@@ -2764,7 +2881,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>614</v>
       </c>
@@ -2772,7 +2889,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>615</v>
       </c>
@@ -2780,7 +2897,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>617</v>
       </c>
@@ -2788,7 +2905,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>618</v>
       </c>
@@ -2796,7 +2913,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>619</v>
       </c>
@@ -2807,7 +2924,7 @@
         <v>619</v>
       </c>
       <c r="D91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E91">
         <v>619</v>
@@ -2816,13 +2933,13 @@
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>620</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E92">
         <v>620</v>
@@ -2831,7 +2948,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>621</v>
       </c>
@@ -2840,10 +2957,10 @@
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>622</v>
       </c>
@@ -2851,19 +2968,19 @@
         <v>622</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>623</v>
       </c>
       <c r="B95" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>624</v>
       </c>
@@ -2871,7 +2988,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>127</v>
       </c>
@@ -2882,6 +2999,1357 @@
       <c r="D98" s="5"/>
       <c r="E98" s="5" t="s">
         <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C1:C98" xr:uid="{5C03F372-2546-4FEA-91D6-CF8178EBED26}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E0C488-9B3B-4341-970D-38839E6B624F}">
+  <dimension ref="A1:G100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="34.44140625" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>101</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>102</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>103</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>104</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>105</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>106</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>107</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>108</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>109</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>110</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>111</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>112</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="G12" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>113</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>114</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>201</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>202</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>203</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>204</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>205</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>206</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>207</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>208</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>209</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>210</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="G24" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>211</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>212</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>214</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>215</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>216</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>302</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>304</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32">
+        <v>305</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33">
+        <v>306</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34">
+        <v>307</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35">
+        <v>308</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36">
+        <v>309</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37">
+        <v>310</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38">
+        <v>311</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39">
+        <v>312</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40">
+        <v>313</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41">
+        <v>314</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42">
+        <v>315</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43">
+        <v>317</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44">
+        <v>318</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45">
+        <v>401</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46">
+        <v>403</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47">
+        <v>404</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48">
+        <v>405</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48">
+        <v>405</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49">
+        <v>406</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50">
+        <v>407</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51">
+        <v>408</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52">
+        <v>410</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="G52" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53">
+        <v>411</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54">
+        <v>412</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55">
+        <v>413</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56">
+        <v>414</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E56">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>415</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58">
+        <v>416</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59">
+        <v>417</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60">
+        <v>418</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61">
+        <v>419</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62">
+        <v>420</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E62">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63">
+        <v>501</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E63">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64">
+        <v>502</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65">
+        <v>503</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E65">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="D66" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E66">
+        <v>504</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67">
+        <v>505</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E67">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68">
+        <v>506</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E68">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69">
+        <v>507</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E69">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B70">
+        <v>508</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71">
+        <v>509</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72">
+        <v>510</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E72">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73">
+        <v>511</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E73">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74">
+        <v>513</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E74">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75">
+        <v>601</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E75">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B76">
+        <v>602</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E76">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77">
+        <v>603</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E77">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78">
+        <v>604</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E78">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79">
+        <v>605</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E79">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B80">
+        <v>606</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="G80" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81">
+        <v>607</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E81">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82">
+        <v>608</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E82">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B83">
+        <v>610</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E83">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84">
+        <v>611</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E84">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B85">
+        <v>612</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86">
+        <v>613</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E86">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87">
+        <v>614</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E87">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88">
+        <v>615</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E88">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89">
+        <v>617</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E89">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90">
+        <v>618</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E90">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91">
+        <v>619</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E91">
+        <v>619</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92">
+        <v>620</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B93">
+        <v>621</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="G93" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B94">
+        <v>622</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E94">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="2"/>
+      <c r="B95">
+        <v>623</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B96">
+        <v>624</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="E96">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C100" s="15"/>
+      <c r="D100" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G100" s="14" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missing ids wave 3 check
</commit_message>
<xml_diff>
--- a/scripts/mssing ids.xlsx
+++ b/scripts/mssing ids.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E059E4A4-2F0A-4931-BF19-787BE47E8F48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654AD711-FD2F-4E98-8994-03515C8F8B4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parent" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="167">
   <si>
     <t>101_1</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>no w2 data. Logs indicate complete assessment at home</t>
+  </si>
+  <si>
+    <t>613 (false start)</t>
+  </si>
+  <si>
+    <t>this is a false start (R_2uUNENaFPEhYnLd)</t>
   </si>
 </sst>
 </file>
@@ -648,16 +654,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -933,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G138"/>
+  <dimension ref="B1:P138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P127" sqref="P127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,87 +941,123 @@
     <col min="5" max="5" width="17.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>107</v>
+      </c>
+      <c r="O7" s="1">
+        <v>107</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1043,8 +1076,11 @@
       <c r="G11" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1063,16 +1099,22 @@
       <c r="G12" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
@@ -1086,8 +1128,9 @@
       <c r="G14" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1099,8 +1142,9 @@
       <c r="G15" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1114,8 +1158,11 @@
       <c r="G16" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
@@ -1129,112 +1176,152 @@
       <c r="G17" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N23">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="D24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>26</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>28</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>30</v>
       </c>
@@ -1242,8 +1329,9 @@
       <c r="E31" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="2:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
         <v>31</v>
       </c>
@@ -1256,216 +1344,295 @@
       <c r="G32" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N33">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N34">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N36">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>36</v>
       </c>
       <c r="D37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N37">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N38">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N39">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>39</v>
       </c>
       <c r="D40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N40">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N41">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N42">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
         <v>42</v>
       </c>
       <c r="D43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N43">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N44">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
         <v>44</v>
       </c>
       <c r="D45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N45">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N46">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>46</v>
       </c>
       <c r="D47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N48">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B49" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N49">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B50" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N50">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B51" s="7" t="s">
         <v>50</v>
       </c>
       <c r="D51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N51">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B52" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N52">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N53">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B54" s="7" t="s">
         <v>53</v>
       </c>
       <c r="D54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N54">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B55" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N55">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B56" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N56">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N57">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B58" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N58">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B59" s="7" t="s">
         <v>58</v>
       </c>
@@ -1473,8 +1640,9 @@
       <c r="E59" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>59</v>
       </c>
@@ -1485,16 +1653,22 @@
       <c r="F60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N60">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B61" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N61">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
         <v>61</v>
       </c>
@@ -1506,24 +1680,31 @@
       <c r="G62" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N62" s="2"/>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>62</v>
       </c>
       <c r="D63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N63">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B64" s="7" t="s">
         <v>63</v>
       </c>
       <c r="D64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N64">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B65" s="7" t="s">
         <v>64</v>
       </c>
@@ -1533,104 +1714,143 @@
       <c r="E65" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N65">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B66" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N66">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B67" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N67">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B68" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N68">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B69" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N69">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>69</v>
       </c>
       <c r="D70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N70">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>70</v>
       </c>
       <c r="D71" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N71">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>71</v>
       </c>
       <c r="D72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N72">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B73" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N73">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B74" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N74">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B75" s="7" t="s">
         <v>74</v>
       </c>
       <c r="D75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N75">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B76" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D76" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N76">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>76</v>
       </c>
       <c r="D77" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N77">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B78" s="7" t="s">
         <v>77</v>
       </c>
@@ -1642,104 +1862,139 @@
       <c r="G78" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N78" s="2"/>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B79" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N79">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B80" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N80">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>80</v>
       </c>
       <c r="D81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N81">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B82" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N82">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B83" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D83" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N83">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>83</v>
       </c>
       <c r="D84" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N84">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B85" s="7" t="s">
         <v>84</v>
       </c>
       <c r="D85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N85">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B86" s="7" t="s">
         <v>85</v>
       </c>
       <c r="D86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N86">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>86</v>
       </c>
       <c r="D87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N87" s="2"/>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B88" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N88">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>88</v>
       </c>
       <c r="D89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N89">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B90" s="7" t="s">
         <v>89</v>
       </c>
       <c r="D90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N90">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B91" s="7" t="s">
         <v>90</v>
       </c>
@@ -1751,8 +2006,9 @@
       <c r="G91" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N91" s="2"/>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B92" s="7" t="s">
         <v>91</v>
       </c>
@@ -1760,8 +2016,9 @@
       <c r="E92" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N92" s="2"/>
+    </row>
+    <row r="93" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>92</v>
       </c>
@@ -1769,80 +2026,108 @@
       <c r="E93" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N93" s="2"/>
+    </row>
+    <row r="94" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B94" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N94">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="95" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B95" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N95">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="96" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B96" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N96">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>96</v>
       </c>
       <c r="D97" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N97">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="98" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B98" s="7" t="s">
         <v>97</v>
       </c>
       <c r="D98" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N98">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="99" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B99" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N99">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="100" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B100" s="7" t="s">
         <v>99</v>
       </c>
       <c r="D100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N100">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="101" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B101" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N101">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="102" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B102" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N102">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="103" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B103" s="7" t="s">
         <v>102</v>
       </c>
@@ -1859,64 +2144,86 @@
       <c r="G103" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N103" s="2"/>
+    </row>
+    <row r="104" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B104" s="7" t="s">
         <v>103</v>
       </c>
       <c r="D104" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N104">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="105" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>104</v>
       </c>
       <c r="D105" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N105">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="106" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>105</v>
       </c>
       <c r="D106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N106">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="107" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B107" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D107" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N107">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="108" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>107</v>
       </c>
       <c r="D108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N108">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="109" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B109" s="7" t="s">
         <v>108</v>
       </c>
       <c r="D109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N109">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="110" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B110" s="7" t="s">
         <v>109</v>
       </c>
       <c r="D110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N110">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="111" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B111" s="7" t="s">
         <v>110</v>
       </c>
@@ -1930,72 +2237,100 @@
       <c r="G111" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N111">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="112" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>111</v>
       </c>
       <c r="D112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N112">
+        <v>613</v>
+      </c>
+      <c r="O112" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B113" s="7" t="s">
         <v>112</v>
       </c>
       <c r="D113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N113">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="114" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B114" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D114" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N114" s="2"/>
+    </row>
+    <row r="115" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>114</v>
       </c>
       <c r="D115" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N115">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="116" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B116" s="7" t="s">
         <v>115</v>
       </c>
       <c r="D116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N116">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="117" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>116</v>
       </c>
       <c r="D117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N117">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="118" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B118" s="7" t="s">
         <v>117</v>
       </c>
       <c r="D118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N118">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="119" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B119" s="7" t="s">
         <v>118</v>
       </c>
       <c r="D119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N119">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="120" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B120" s="7" t="s">
         <v>119</v>
       </c>
@@ -2014,8 +2349,11 @@
       <c r="G120" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N120">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="121" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B121" s="7" t="s">
         <v>120</v>
       </c>
@@ -2032,8 +2370,11 @@
       <c r="G121" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N121">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="122" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B122" s="7" t="s">
         <v>121</v>
       </c>
@@ -2046,16 +2387,20 @@
       <c r="E122" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N122" s="2"/>
+    </row>
+    <row r="123" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B123" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N123">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="124" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B124" s="2"/>
       <c r="C124" t="s">
         <v>152</v>
@@ -2064,16 +2409,20 @@
       <c r="E124" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N124" s="2"/>
+    </row>
+    <row r="125" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B125" s="7" t="s">
         <v>123</v>
       </c>
       <c r="D125" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="N125">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="127" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B127" s="5" t="s">
         <v>124</v>
       </c>
@@ -2097,9 +2446,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:E137" xr:uid="{3C1546A2-BF81-4539-8024-42C8CDD12298}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2107,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3011,13 +3359,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E0C488-9B3B-4341-970D-38839E6B624F}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="I58" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="34.44140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="28.44140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
initial cleaning wave 3
</commit_message>
<xml_diff>
--- a/scripts/mssing ids.xlsx
+++ b/scripts/mssing ids.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654AD711-FD2F-4E98-8994-03515C8F8B4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B087D3-7D63-411C-BEE0-14B6BDB7FFDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
     <t>613 (false start)</t>
   </si>
   <si>
-    <t>this is a false start (R_2uUNENaFPEhYnLd)</t>
+    <t>has -99 throughout (R_2uUNENaFPEhYnLd)</t>
   </si>
 </sst>
 </file>
@@ -933,7 +933,7 @@
   <dimension ref="B1:P138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P127" sqref="P127"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3359,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E0C488-9B3B-4341-970D-38839E6B624F}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="I58" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
parent wave 3 completed. Confirmation pending about my conclusion.
</commit_message>
<xml_diff>
--- a/scripts/mssing ids.xlsx
+++ b/scripts/mssing ids.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B087D3-7D63-411C-BEE0-14B6BDB7FFDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6464CC7F-2C7B-4943-8819-D741EA700DC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="171">
   <si>
     <t>101_1</t>
   </si>
@@ -528,6 +528,18 @@
   </si>
   <si>
     <t>has -99 throughout (R_2uUNENaFPEhYnLd)</t>
+  </si>
+  <si>
+    <t>408 says imported</t>
+  </si>
+  <si>
+    <t>405 says imported</t>
+  </si>
+  <si>
+    <t>dupes</t>
+  </si>
+  <si>
+    <t>says imported, but it's not duplicated</t>
   </si>
 </sst>
 </file>
@@ -933,7 +945,7 @@
   <dimension ref="B1:P138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1534,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B49" s="7" t="s">
         <v>48</v>
       </c>
@@ -1533,7 +1545,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B50" s="7" t="s">
         <v>49</v>
       </c>
@@ -1544,7 +1556,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B51" s="7" t="s">
         <v>50</v>
       </c>
@@ -1555,7 +1567,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B52" s="7" t="s">
         <v>51</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
         <v>52</v>
       </c>
@@ -1577,7 +1589,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B54" s="7" t="s">
         <v>53</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B55" s="7" t="s">
         <v>54</v>
       </c>
@@ -1599,7 +1611,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B56" s="7" t="s">
         <v>55</v>
       </c>
@@ -1610,7 +1622,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
         <v>56</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B58" s="7" t="s">
         <v>57</v>
       </c>
@@ -1632,7 +1644,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B59" s="7" t="s">
         <v>58</v>
       </c>
@@ -1642,7 +1654,7 @@
       </c>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>59</v>
       </c>
@@ -1656,8 +1668,11 @@
       <c r="N60">
         <v>405</v>
       </c>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="O60" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B61" s="7" t="s">
         <v>60</v>
       </c>
@@ -1668,7 +1683,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
         <v>61</v>
       </c>
@@ -1682,7 +1697,7 @@
       </c>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>62</v>
       </c>
@@ -1693,7 +1708,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B64" s="7" t="s">
         <v>63</v>
       </c>
@@ -1702,6 +1717,9 @@
       </c>
       <c r="N64">
         <v>408</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.3">
@@ -2082,6 +2100,9 @@
       <c r="N98">
         <v>601</v>
       </c>
+      <c r="O98" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B99" s="7" t="s">
@@ -2251,11 +2272,11 @@
       <c r="N112">
         <v>613</v>
       </c>
-      <c r="O112" t="s">
+      <c r="O112" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B113" s="7" t="s">
         <v>112</v>
       </c>
@@ -2266,7 +2287,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="114" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B114" s="7" t="s">
         <v>113</v>
       </c>
@@ -2275,7 +2296,7 @@
       </c>
       <c r="N114" s="2"/>
     </row>
-    <row r="115" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>114</v>
       </c>
@@ -2286,7 +2307,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="116" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B116" s="7" t="s">
         <v>115</v>
       </c>
@@ -2297,7 +2318,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="117" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>116</v>
       </c>
@@ -2308,7 +2329,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="118" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B118" s="7" t="s">
         <v>117</v>
       </c>
@@ -2319,7 +2340,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="119" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B119" s="7" t="s">
         <v>118</v>
       </c>
@@ -2330,7 +2351,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="120" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B120" s="7" t="s">
         <v>119</v>
       </c>
@@ -2353,7 +2374,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B121" s="7" t="s">
         <v>120</v>
       </c>
@@ -2374,7 +2395,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="122" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B122" s="7" t="s">
         <v>121</v>
       </c>
@@ -2389,7 +2410,7 @@
       </c>
       <c r="N122" s="2"/>
     </row>
-    <row r="123" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B123" s="7" t="s">
         <v>122</v>
       </c>
@@ -2400,7 +2421,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="124" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B124" s="2"/>
       <c r="C124" t="s">
         <v>152</v>
@@ -2411,7 +2432,7 @@
       </c>
       <c r="N124" s="2"/>
     </row>
-    <row r="125" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B125" s="7" t="s">
         <v>123</v>
       </c>
@@ -2422,7 +2443,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="127" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B127" s="5" t="s">
         <v>124</v>
       </c>
@@ -2433,6 +2454,9 @@
       <c r="E127" s="6"/>
       <c r="F127" s="5" t="s">
         <v>154</v>
+      </c>
+      <c r="O127" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.3">
@@ -2455,8 +2479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3359,8 +3383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3E0C488-9B3B-4341-970D-38839E6B624F}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N90" sqref="N90"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J108" sqref="J108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Some progresss on scales
</commit_message>
<xml_diff>
--- a/scripts/mssing ids.xlsx
+++ b/scripts/mssing ids.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="parent" sheetId="1" r:id="rId1"/>
     <sheet name="youth" sheetId="2" r:id="rId2"/>
     <sheet name="parent &amp; youth" sheetId="3" r:id="rId3"/>
     <sheet name="parent 3 waves" sheetId="5" r:id="rId4"/>
-    <sheet name="youth 3 waves" sheetId="4" r:id="rId5"/>
+    <sheet name="Primary caregivers only" sheetId="6" r:id="rId5"/>
+    <sheet name="youth 3 waves" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">parent!$N$1:$N$138</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="183">
   <si>
     <t>101_1</t>
   </si>
@@ -575,13 +576,16 @@
   </si>
   <si>
     <t>removing participants with just 1 wave (red highlight)</t>
+  </si>
+  <si>
+    <t>choose father, not mother, has more waves of data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,6 +612,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -666,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -698,6 +714,23 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4783,15 +4816,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="9.140625" style="22"/>
+    <col min="11" max="11" width="9.140625" style="23"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4801,8 +4838,9 @@
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -4812,8 +4850,10 @@
       <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J2" s="20"/>
+      <c r="K2" s="24"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -4823,8 +4863,10 @@
       <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J3" s="20"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -4834,8 +4876,10 @@
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J4" s="20"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -4845,8 +4889,10 @@
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J5" s="20"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -4856,8 +4902,10 @@
       <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J6" s="20"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -4867,8 +4915,10 @@
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J7" s="20"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -4878,8 +4928,10 @@
       <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J8" s="20"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -4889,8 +4941,10 @@
       <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J9" s="20"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4900,24 +4954,30 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J10" s="20"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J11" s="20"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J12" s="20"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -4927,37 +4987,47 @@
       <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J13" s="20"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J14" s="20"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J15" s="20"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J16" s="20"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J17" s="20"/>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
@@ -4967,8 +5037,10 @@
       <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J18" s="20"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
@@ -4978,30 +5050,36 @@
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="J19" s="20"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="J20" s="20"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J21" s="20"/>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
@@ -5011,8 +5089,10 @@
       <c r="C22" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J22" s="20"/>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
@@ -5022,8 +5102,10 @@
       <c r="C23" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J23" s="20"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -5033,8 +5115,10 @@
       <c r="C24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J24" s="20"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>24</v>
       </c>
@@ -5044,8 +5128,10 @@
       <c r="C25" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J25" s="20"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
@@ -5055,8 +5141,10 @@
       <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J26" s="20"/>
+      <c r="K26" s="24"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -5066,8 +5154,10 @@
       <c r="C27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J27" s="20"/>
+      <c r="K27" s="24"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>27</v>
       </c>
@@ -5077,16 +5167,20 @@
       <c r="C28" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J28" s="20"/>
+      <c r="K28" s="24"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J29" s="20"/>
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>29</v>
       </c>
@@ -5096,13 +5190,17 @@
       <c r="C30" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J30" s="20"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J31" s="20"/>
+      <c r="K31" s="24"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>31</v>
       </c>
@@ -5112,8 +5210,10 @@
       <c r="C32" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J32" s="20"/>
+      <c r="K32" s="24"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>32</v>
       </c>
@@ -5123,8 +5223,10 @@
       <c r="C33" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J33" s="20"/>
+      <c r="K33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>33</v>
       </c>
@@ -5134,8 +5236,10 @@
       <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J34" s="20"/>
+      <c r="K34" s="24"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>34</v>
       </c>
@@ -5145,8 +5249,10 @@
       <c r="C35" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J35" s="20"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>35</v>
       </c>
@@ -5156,8 +5262,10 @@
       <c r="C36" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J36" s="20"/>
+      <c r="K36" s="24"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>37</v>
       </c>
@@ -5167,8 +5275,10 @@
       <c r="C37" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J37" s="20"/>
+      <c r="K37" s="24"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -5178,8 +5288,10 @@
       <c r="C38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J38" s="20"/>
+      <c r="K38" s="24"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>38</v>
       </c>
@@ -5189,8 +5301,10 @@
       <c r="C39" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J39" s="20"/>
+      <c r="K39" s="24"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -5200,8 +5314,10 @@
       <c r="C40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J40" s="20"/>
+      <c r="K40" s="24"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>40</v>
       </c>
@@ -5211,8 +5327,10 @@
       <c r="C41" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J41" s="20"/>
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
@@ -5222,8 +5340,10 @@
       <c r="C42" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J42" s="20"/>
+      <c r="K42" s="24"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>42</v>
       </c>
@@ -5233,8 +5353,10 @@
       <c r="C43" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J43" s="20"/>
+      <c r="K43" s="24"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>43</v>
       </c>
@@ -5244,8 +5366,10 @@
       <c r="C44" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J44" s="20"/>
+      <c r="K44" s="24"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>44</v>
       </c>
@@ -5255,8 +5379,10 @@
       <c r="C45" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J45" s="20"/>
+      <c r="K45" s="24"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>45</v>
       </c>
@@ -5266,8 +5392,10 @@
       <c r="C46" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J46" s="20"/>
+      <c r="K46" s="24"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>47</v>
       </c>
@@ -5275,16 +5403,20 @@
         <v>47</v>
       </c>
       <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J47" s="20"/>
+      <c r="K47" s="24"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J48" s="20"/>
+      <c r="K48" s="24"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>48</v>
       </c>
@@ -5294,8 +5426,10 @@
       <c r="C49" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J49" s="20"/>
+      <c r="K49" s="24"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>49</v>
       </c>
@@ -5305,8 +5439,10 @@
       <c r="C50" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J50" s="20"/>
+      <c r="K50" s="24"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>50</v>
       </c>
@@ -5316,8 +5452,10 @@
       <c r="C51" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J51" s="20"/>
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>51</v>
       </c>
@@ -5327,8 +5465,10 @@
       <c r="C52" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J52" s="20"/>
+      <c r="K52" s="24"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>52</v>
       </c>
@@ -5338,8 +5478,10 @@
       <c r="C53" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J53" s="20"/>
+      <c r="K53" s="24"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>53</v>
       </c>
@@ -5349,8 +5491,10 @@
       <c r="C54" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J54" s="20"/>
+      <c r="K54" s="24"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>54</v>
       </c>
@@ -5360,8 +5504,10 @@
       <c r="C55" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J55" s="20"/>
+      <c r="K55" s="24"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>55</v>
       </c>
@@ -5371,8 +5517,10 @@
       <c r="C56" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J56" s="20"/>
+      <c r="K56" s="24"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>56</v>
       </c>
@@ -5382,8 +5530,10 @@
       <c r="C57" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J57" s="20"/>
+      <c r="K57" s="24"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>57</v>
       </c>
@@ -5393,13 +5543,17 @@
       <c r="C58" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J58" s="20"/>
+      <c r="K58" s="24"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J59" s="20"/>
+      <c r="K59" s="24"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>59</v>
       </c>
@@ -5407,8 +5561,13 @@
       <c r="C60" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>182</v>
+      </c>
+      <c r="J60" s="20"/>
+      <c r="K60" s="24"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>60</v>
       </c>
@@ -5418,13 +5577,17 @@
       <c r="C61" s="7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J61" s="20"/>
+      <c r="K61" s="24"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J62" s="20"/>
+      <c r="K62" s="24"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>63</v>
       </c>
@@ -5434,8 +5597,10 @@
       <c r="C63" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J63" s="20"/>
+      <c r="K63" s="24"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -5445,8 +5610,10 @@
       <c r="C64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J64" s="20"/>
+      <c r="K64" s="24"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>64</v>
       </c>
@@ -5456,8 +5623,10 @@
       <c r="C65" s="7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J65" s="20"/>
+      <c r="K65" s="24"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>65</v>
       </c>
@@ -5467,8 +5636,10 @@
       <c r="C66" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J66" s="20"/>
+      <c r="K66" s="24"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>66</v>
       </c>
@@ -5478,8 +5649,10 @@
       <c r="C67" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J67" s="20"/>
+      <c r="K67" s="24"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>67</v>
       </c>
@@ -5489,8 +5662,10 @@
       <c r="C68" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J68" s="20"/>
+      <c r="K68" s="24"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>68</v>
       </c>
@@ -5500,19 +5675,23 @@
       <c r="C69" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
+      <c r="J69" s="20"/>
+      <c r="K69" s="24"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J70" s="20"/>
+      <c r="K70" s="24"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>72</v>
       </c>
@@ -5522,8 +5701,10 @@
       <c r="C71" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J71" s="20"/>
+      <c r="K71" s="24"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -5533,8 +5714,10 @@
       <c r="C72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J72" s="20"/>
+      <c r="K72" s="24"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -5544,8 +5727,10 @@
       <c r="C73" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J73" s="20"/>
+      <c r="K73" s="24"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>73</v>
       </c>
@@ -5555,8 +5740,10 @@
       <c r="C74" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J74" s="20"/>
+      <c r="K74" s="24"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>74</v>
       </c>
@@ -5566,8 +5753,10 @@
       <c r="C75" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J75" s="20"/>
+      <c r="K75" s="24"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>75</v>
       </c>
@@ -5577,8 +5766,10 @@
       <c r="C76" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J76" s="20"/>
+      <c r="K76" s="24"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -5588,13 +5779,17 @@
       <c r="C77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J77" s="20"/>
+      <c r="K77" s="24"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J78" s="20"/>
+      <c r="K78" s="24"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>78</v>
       </c>
@@ -5604,8 +5799,10 @@
       <c r="C79" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J79" s="20"/>
+      <c r="K79" s="24"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>79</v>
       </c>
@@ -5615,8 +5812,10 @@
       <c r="C80" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J80" s="20"/>
+      <c r="K80" s="24"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -5626,8 +5825,10 @@
       <c r="C81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J81" s="20"/>
+      <c r="K81" s="24"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>81</v>
       </c>
@@ -5637,8 +5838,10 @@
       <c r="C82" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J82" s="20"/>
+      <c r="K82" s="24"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>82</v>
       </c>
@@ -5648,8 +5851,10 @@
       <c r="C83" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J83" s="20"/>
+      <c r="K83" s="24"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -5659,8 +5864,10 @@
       <c r="C84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J84" s="20"/>
+      <c r="K84" s="24"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>84</v>
       </c>
@@ -5670,8 +5877,10 @@
       <c r="C85" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J85" s="20"/>
+      <c r="K85" s="24"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>85</v>
       </c>
@@ -5681,16 +5890,20 @@
       <c r="C86" s="7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J86" s="20"/>
+      <c r="K86" s="24"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J87" s="20"/>
+      <c r="K87" s="24"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>87</v>
       </c>
@@ -5700,8 +5913,10 @@
       <c r="C88" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J88" s="20"/>
+      <c r="K88" s="24"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -5711,8 +5926,10 @@
       <c r="C89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J89" s="20"/>
+      <c r="K89" s="24"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>89</v>
       </c>
@@ -5722,23 +5939,31 @@
       <c r="C90" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J90" s="20"/>
+      <c r="K90" s="24"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J91" s="20"/>
+      <c r="K91" s="24"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J92" s="20"/>
+      <c r="K92" s="24"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J93" s="20"/>
+      <c r="K93" s="24"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>93</v>
       </c>
@@ -5748,8 +5973,10 @@
       <c r="C94" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J94" s="20"/>
+      <c r="K94" s="24"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>94</v>
       </c>
@@ -5759,8 +5986,10 @@
       <c r="C95" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="J95" s="20"/>
+      <c r="K95" s="24"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>95</v>
       </c>
@@ -5770,6 +5999,8 @@
       <c r="C96" s="7" t="s">
         <v>95</v>
       </c>
+      <c r="J96" s="21"/>
+      <c r="K96" s="24"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
@@ -5972,6 +6203,9 @@
       <c r="C115" s="7" t="s">
         <v>114</v>
       </c>
+      <c r="D115" s="7" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
@@ -6092,6 +6326,505 @@
       </c>
       <c r="D129" t="s">
         <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="25" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -6099,12 +6832,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>